<commit_message>
starting on other files
</commit_message>
<xml_diff>
--- a/loc.xlsx
+++ b/loc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyDocuments\dv\Github\PDCurses\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3574FB8F-4AEA-4825-9501-1ABBDCED4275}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C35ECA0-DBBA-47C1-A2A1-CB47B33438A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A8AC9413-688C-4E95-8E2D-974077D7ABE3}"/>
+    <workbookView xWindow="43650" yWindow="120" windowWidth="17865" windowHeight="15435" xr2:uid="{A8AC9413-688C-4E95-8E2D-974077D7ABE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>addch</t>
   </si>
@@ -183,6 +183,12 @@
   </si>
   <si>
     <t>File</t>
+  </si>
+  <si>
+    <t>DONE</t>
+  </si>
+  <si>
+    <t>started</t>
   </si>
 </sst>
 </file>
@@ -554,23 +560,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5888984-75EE-47A5-BF9D-297DAF2EC4E8}">
-  <dimension ref="A2:C52"/>
+  <dimension ref="A2:D52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>48</v>
       </c>
       <c r="C2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -581,7 +590,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -592,7 +601,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -603,7 +612,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -614,18 +623,18 @@
         <v>411</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>4</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>76</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -636,7 +645,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -647,7 +656,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -658,7 +667,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -669,7 +678,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -680,7 +689,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -691,7 +700,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -702,7 +711,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -713,7 +722,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -724,7 +733,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -735,7 +744,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
@@ -746,7 +755,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
@@ -757,7 +766,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
@@ -768,7 +777,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
@@ -779,7 +788,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
@@ -790,7 +799,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
@@ -801,7 +810,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
@@ -812,7 +821,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
@@ -823,7 +832,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
@@ -834,7 +843,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>25</v>
       </c>
@@ -845,7 +854,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>26</v>
       </c>
@@ -855,8 +864,11 @@
       <c r="C28">
         <v>79</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D28" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>27</v>
       </c>
@@ -867,7 +879,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>28</v>
       </c>
@@ -878,7 +890,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>29</v>
       </c>
@@ -889,7 +901,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>30</v>
       </c>
@@ -1065,7 +1077,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>46</v>
       </c>
@@ -1076,7 +1088,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>47</v>
       </c>
@@ -1087,10 +1099,14 @@
         <v>26</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C52">
         <f>SUM(C3:C51)</f>
-        <v>13887</v>
+        <v>13811</v>
+      </c>
+      <c r="D52">
+        <f>SUM(D3:D51)</f>
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>